<commit_message>
error catching forexcel upload
</commit_message>
<xml_diff>
--- a/public/jobs/excel/libreimport.xlsx
+++ b/public/jobs/excel/libreimport.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>first_name</t>
   </si>
@@ -42,6 +42,18 @@
   </si>
   <si>
     <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>fgdg</t>
+  </si>
+  <si>
+    <t>fgd</t>
+  </si>
+  <si>
+    <t>dfgg</t>
+  </si>
+  <si>
+    <t>gg@hh.com</t>
   </si>
 </sst>
 </file>
@@ -168,10 +180,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E6" activeCellId="0" pane="topLeft" sqref="E6"/>
+      <selection activeCell="E3" activeCellId="0" pane="topLeft" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -229,9 +241,27 @@
         <v>8</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink display="test@gmail.com" ref="E2" r:id="rId1"/>
+    <hyperlink display="gg@hh.com" ref="E3" r:id="rId2"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>